<commit_message>
[맘파] ObjectTable, RecipeTable 수정 업데이트
</commit_message>
<xml_diff>
--- a/ExcelConverter/ExcelFiles/RecipeTable.xlsx
+++ b/ExcelConverter/ExcelFiles/RecipeTable.xlsx
@@ -3839,8 +3839,8 @@
       <c r="F10" s="8">
         <v>10.0</v>
       </c>
-      <c r="G10" s="8">
-        <v>2.0</v>
+      <c r="G10" s="15">
+        <v>1002.0</v>
       </c>
       <c r="H10" s="8">
         <v>42.0</v>
@@ -3877,8 +3877,8 @@
       <c r="F11" s="8">
         <v>14.0</v>
       </c>
-      <c r="G11" s="8">
-        <v>2.0</v>
+      <c r="G11" s="15">
+        <v>1002.0</v>
       </c>
       <c r="H11" s="8">
         <v>45.0</v>
@@ -3915,8 +3915,8 @@
       <c r="F12" s="8">
         <v>15.0</v>
       </c>
-      <c r="G12" s="8">
-        <v>2.0</v>
+      <c r="G12" s="15">
+        <v>1002.0</v>
       </c>
       <c r="H12" s="8">
         <v>57.0</v>
@@ -3953,8 +3953,8 @@
       <c r="F13" s="8">
         <v>17.0</v>
       </c>
-      <c r="G13" s="8">
-        <v>2.0</v>
+      <c r="G13" s="15">
+        <v>1002.0</v>
       </c>
       <c r="H13" s="8">
         <v>63.0</v>
@@ -3991,8 +3991,8 @@
       <c r="F14" s="8">
         <v>8.0</v>
       </c>
-      <c r="G14" s="8">
-        <v>2.0</v>
+      <c r="G14" s="15">
+        <v>1002.0</v>
       </c>
       <c r="H14" s="8">
         <v>40.0</v>
@@ -4029,8 +4029,8 @@
       <c r="F15" s="8">
         <v>12.0</v>
       </c>
-      <c r="G15" s="8">
-        <v>2.0</v>
+      <c r="G15" s="15">
+        <v>1002.0</v>
       </c>
       <c r="H15" s="8">
         <v>44.0</v>
@@ -4067,8 +4067,8 @@
       <c r="F16" s="8">
         <v>16.0</v>
       </c>
-      <c r="G16" s="8">
-        <v>2.0</v>
+      <c r="G16" s="15">
+        <v>1002.0</v>
       </c>
       <c r="H16" s="8">
         <v>62.0</v>
@@ -4105,8 +4105,8 @@
       <c r="F17" s="8">
         <v>9.0</v>
       </c>
-      <c r="G17" s="8">
-        <v>7.0</v>
+      <c r="G17" s="15">
+        <v>1007.0</v>
       </c>
       <c r="H17" s="8">
         <v>28.0</v>

</xml_diff>